<commit_message>
added the employee details and generated pay slip for each employee
</commit_message>
<xml_diff>
--- a/BANK LETTER.xlsx
+++ b/BANK LETTER.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1125" windowWidth="19470" windowHeight="7935" firstSheet="15" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="1125" windowWidth="15300" windowHeight="4860" firstSheet="17" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">Sheet3!$A$1:$H$46</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A11:J24"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1224,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3552,8 +3552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A13:E47"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A16" zoomScale="60" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5379,8 +5379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A13:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>